<commit_message>
Modify the Excel file and regenerate
This works well, so this scaffolding project now works.

The Excel file now contains a calculation for the sum, which is hopefully a
nice example of using the power of excel when defining the tests.
</commit_message>
<xml_diff>
--- a/CustomerTests/ExcelTests/Sum.xlsx
+++ b/CustomerTests/ExcelTests/Sum.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel-sample-usage\SutTests\ExcelTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel-sample-usage\CustomerTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0A1A7C-6FDA-478E-8C01-E940D234DA5E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD43BF2-DB64-4911-BC60-D98F7AE3B37A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sum 1 and 2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sum 1 and 3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -48,9 +48,6 @@
     <t>Calculator</t>
   </si>
   <si>
-    <t>Sum 1 and 2</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>Y of</t>
+  </si>
+  <si>
+    <t>Sum 1 and 3</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -521,7 +521,7 @@
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -531,10 +531,10 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -552,13 +552,14 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <f>D5+D6</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add conditional formatting rules to excel sheets
These format the various bits of the test automatically
</commit_message>
<xml_diff>
--- a/CustomerTests/ExcelTests/Sum.xlsx
+++ b/CustomerTests/ExcelTests/Sum.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel-sample-usage\CustomerTests\ExcelTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel-scaffolding\CustomerTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD43BF2-DB64-4911-BC60-D98F7AE3B37A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573CC9C7-F2CA-43F4-9225-6F8664A584BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,56 +75,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,42 +93,102 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
-    <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
-    <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
-    <cellStyle name="40% - Accent6" xfId="5" builtinId="51"/>
-    <cellStyle name="Accent4" xfId="1" builtinId="41"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -484,56 +501,50 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="1">
         <v>3</v>
       </c>
     </row>
@@ -541,7 +552,7 @@
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -551,18 +562,52 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f>D5+D6</f>
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="5" operator="beginsWith" text="With Properties">
+      <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="4" priority="6" operator="endsWith" text=" table of">
+      <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="3" priority="7" operator="endsWith" text=" of">
+      <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="10">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove trailing space in excel
</commit_message>
<xml_diff>
--- a/CustomerTests/ExcelTests/Sum.xlsx
+++ b/CustomerTests/ExcelTests/Sum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel-scaffolding\CustomerTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573CC9C7-F2CA-43F4-9225-6F8664A584BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320C268D-7B8B-464E-A95E-66E03A8492C6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>=</t>
   </si>
   <si>
-    <t xml:space="preserve">Result </t>
-  </si>
-  <si>
     <t>X of</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>Sum 1 and 3</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,7 +534,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>

</xml_diff>